<commit_message>
Changed variable name and description in excel file
</commit_message>
<xml_diff>
--- a/Data/Codebook/Codebook_OOP.xlsx
+++ b/Data/Codebook/Codebook_OOP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SESS-Paper-Writing\OOP-Analysis\Data\Codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59DADCD-F180-4F28-891B-8D97FCFD58C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DB88DC-CAD1-413A-9BB4-35ED4AA8D980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2EED559F-E636-4A0E-939A-E1AF51D2816F}"/>
   </bookViews>
@@ -118,9 +118,6 @@
     <t>The marital status of the head of the household.</t>
   </si>
   <si>
-    <t>The presence of chronic illnesses within a household.</t>
-  </si>
-  <si>
     <t>The type of health facility a household has access to.</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>The total annual consumption expenditure of a household for durable goods.</t>
+  </si>
+  <si>
+    <t>The presence of Hepatitus B &amp; C within a household (proxy for chronic illnesses).</t>
   </si>
 </sst>
 </file>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7750F2DE-785C-40AF-948A-856B205FC231}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,13 +745,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
@@ -768,7 +768,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>21</v>
@@ -783,7 +783,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>21</v>
@@ -811,7 +811,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>21</v>
@@ -826,7 +826,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>21</v>
@@ -837,13 +837,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>21</v>
@@ -852,10 +852,10 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="3"/>
@@ -866,10 +866,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>21</v>
@@ -880,13 +880,13 @@
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="D11" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>21</v>
@@ -898,10 +898,10 @@
         <v>16</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>21</v>
@@ -915,10 +915,10 @@
         <v>18</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>21</v>
@@ -930,10 +930,10 @@
         <v>19</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>21</v>
@@ -945,10 +945,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>21</v>

</xml_diff>